<commit_message>
Distortion correction works now.
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\Windows\SteamVR-Undistort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Windows\SteamVR-Undistort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAA821C1-0C5A-494D-A6D5-778ACC216AD2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B027E73-1726-49AC-8EDC-54E4A382CE36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{6DC6B09A-E7DA-49A2-B7A4-0C67EEFD1649}"/>
   </bookViews>
@@ -306,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -349,6 +349,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A7B1EB-79F9-4052-A890-3A2B4DC96661}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +723,10 @@
       <c r="F3" s="2"/>
     </row>
     <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>1+H66</f>
+        <v>1.600000023841857</v>
+      </c>
       <c r="G5" s="10" t="s">
         <v>48</v>
       </c>
@@ -733,10 +738,20 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="B6" s="28">
+        <f>G41/B5</f>
+        <v>0.76388887750605672</v>
+      </c>
+      <c r="C6" s="28">
+        <v>0</v>
+      </c>
+      <c r="D6" s="28">
+        <f>I41/B5</f>
+        <v>-5.5808996881410548E-2</v>
+      </c>
+      <c r="E6" s="28">
+        <v>0</v>
+      </c>
       <c r="G6" s="6">
         <v>0.76388883600000002</v>
       </c>
@@ -775,10 +790,20 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="B7" s="28">
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <f>H42/B5</f>
+        <v>0.68749998975545223</v>
+      </c>
+      <c r="D7" s="28">
+        <f>I42/B5</f>
+        <v>1.402465838529675E-3</v>
+      </c>
+      <c r="E7" s="28">
+        <v>0</v>
+      </c>
       <c r="G7" s="6">
         <v>0</v>
       </c>
@@ -817,10 +842,20 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="B8" s="28">
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <v>0</v>
+      </c>
+      <c r="D8" s="28">
+        <f>(0.01+1000)/(0.01-1000)</f>
+        <v>-1.0000200002000019</v>
+      </c>
+      <c r="E8" s="28">
+        <f>(1000*0.01)/(0.01-1000)</f>
+        <v>-1.000010000100001E-2</v>
+      </c>
       <c r="G8" s="6">
         <v>0</v>
       </c>
@@ -859,10 +894,18 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="B9" s="28">
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0</v>
+      </c>
+      <c r="D9" s="28">
+        <v>-1</v>
+      </c>
+      <c r="E9" s="28">
+        <v>0</v>
+      </c>
       <c r="G9" s="6">
         <v>0</v>
       </c>
@@ -1357,6 +1400,10 @@
       <c r="J31" s="7">
         <v>-3.4700000000000002E-2</v>
       </c>
+      <c r="K31">
+        <f>O31-J31</f>
+        <v>6.9400000000000003E-2</v>
+      </c>
       <c r="L31" s="14">
         <v>1</v>
       </c>
@@ -1396,7 +1443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G33" s="7">
         <v>0</v>
       </c>
@@ -1422,7 +1469,17 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f>I6/G41</f>
+        <v>-4.5661923245454622E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <f>I7/H42</f>
+        <v>1.2749434545454544E-3</v>
+      </c>
       <c r="G35" s="11">
         <v>1</v>
       </c>
@@ -1448,7 +1505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G36" s="11">
         <v>0</v>
       </c>
@@ -1474,7 +1531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G37" s="11">
         <v>0</v>
       </c>
@@ -1503,7 +1560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
         <v>43</v>
       </c>
@@ -1511,7 +1568,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f>G41/H42</f>
+        <v>1.1111111111111092</v>
+      </c>
+      <c r="E41">
+        <f>G6/G41</f>
+        <v>0.62499995672727382</v>
+      </c>
       <c r="G41" s="4">
         <v>1.2222222222222201</v>
       </c>
@@ -1531,7 +1596,11 @@
         <v>9.1627463698387104E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f>H7/H42</f>
+        <v>0.62500005454545449</v>
+      </c>
       <c r="G42" s="4">
         <v>0</v>
       </c>
@@ -1551,7 +1620,7 @@
         <v>-7.4033150449395102E-3</v>
       </c>
     </row>
-    <row r="43" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G43" s="4">
         <v>0</v>
       </c>
@@ -1571,7 +1640,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="7:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f>I41*E41</f>
+        <v>-5.5808993849017413E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f>I42*E42</f>
+        <v>1.4024659818250641E-3</v>
+      </c>
       <c r="G45" s="4" t="s">
         <v>52</v>
       </c>
@@ -1590,8 +1669,12 @@
       <c r="N45" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="46" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="P45">
+        <f>N41*E42</f>
+        <v>5.7267169809353591E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G46" s="4">
         <v>0</v>
       </c>
@@ -1610,8 +1693,12 @@
       <c r="N46" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="47" spans="7:15" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <f>N42*E42</f>
+        <v>-4.6270723069043781E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G47" s="4">
         <v>0</v>
       </c>
@@ -1711,8 +1798,8 @@
         <v>490.52116960287094</v>
       </c>
       <c r="N53">
-        <f>M53/M49</f>
-        <v>0.45418626815080643</v>
+        <f>(M53-540)/540</f>
+        <v>-9.1627463698387146E-2</v>
       </c>
     </row>
     <row r="54" spans="7:15" x14ac:dyDescent="0.25">
@@ -1735,8 +1822,8 @@
         <v>595.55801097303629</v>
       </c>
       <c r="N54">
-        <f>M54/M50</f>
-        <v>0.49629834247753024</v>
+        <f>(M54-600)/600</f>
+        <v>-7.403315044939518E-3</v>
       </c>
     </row>
     <row r="56" spans="7:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
merged left and right hand info panels on left hand.
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Windows\SteamVR-Undistort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\Windows\SteamVR-Undistort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B027E73-1726-49AC-8EDC-54E4A382CE36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E7841-D346-4001-9F47-0CD3825A84B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{6DC6B09A-E7DA-49A2-B7A4-0C67EEFD1649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
   <si>
     <t>width</t>
   </si>
@@ -184,13 +185,58 @@
   </si>
   <si>
     <t>2fx/w</t>
+  </si>
+  <si>
+    <t>CenterX</t>
+  </si>
+  <si>
+    <t>CenterY</t>
+  </si>
+  <si>
+    <t>FocalX</t>
+  </si>
+  <si>
+    <t>FocalY</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>Grow</t>
+  </si>
+  <si>
+    <t>CutOff</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Adjust Step</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +254,23 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,8 +313,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -302,11 +399,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -350,6 +460,84 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A7B1EB-79F9-4052-A890-3A2B4DC96661}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,4 +2224,617 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D0AAC0-3998-45C2-B43B-2ADF12A7E90E}">
+  <dimension ref="B1:S29"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="0.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="35" customWidth="1"/>
+    <col min="4" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="0.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="27" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="0.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:19" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="55"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="55"/>
+      <c r="C3" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="32"/>
+      <c r="S3" s="32"/>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="55"/>
+      <c r="C4" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="55"/>
+      <c r="C5" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="R5" s="32"/>
+      <c r="S5" s="32"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="55"/>
+      <c r="C6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="55"/>
+      <c r="C7" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="45"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="32"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="55"/>
+      <c r="C8" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="32"/>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="55"/>
+      <c r="C9" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="30"/>
+      <c r="S9" s="30"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="55"/>
+      <c r="C10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="32"/>
+      <c r="S10" s="32"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="55"/>
+      <c r="C11" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="55"/>
+      <c r="C12" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="30"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="55"/>
+      <c r="C13" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="46"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="32"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="55"/>
+      <c r="C14" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="55"/>
+      <c r="C15" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="55"/>
+      <c r="C16" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="55"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="55"/>
+      <c r="C17" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="55"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="55"/>
+      <c r="C18" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="55"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="55"/>
+      <c r="C19" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="55"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="55"/>
+      <c r="C20" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="55"/>
+      <c r="C21" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="55"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="55"/>
+      <c r="C22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="57"/>
+      <c r="K22" s="27"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="55"/>
+      <c r="C23" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="57"/>
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="55"/>
+      <c r="C24" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="27"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="55"/>
+      <c r="C25" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="55"/>
+      <c r="C26" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="27"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="55"/>
+      <c r="C27" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B28" s="55"/>
+      <c r="C28" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="55"/>
+    </row>
+    <row r="29" spans="2:11" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
+      <c r="J29" s="55"/>
+    </row>
+  </sheetData>
+  <mergeCells count="52">
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added an ugly menu
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\Windows\SteamVR-Undistort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E7841-D346-4001-9F47-0CD3825A84B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A905752-D62A-4422-A146-274A0AB1BC11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{6DC6B09A-E7DA-49A2-B7A4-0C67EEFD1649}"/>
   </bookViews>
@@ -270,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +349,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -416,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -460,9 +466,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -473,9 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -483,28 +483,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -512,31 +491,61 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2231,334 +2240,334 @@
   <dimension ref="B1:S29"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="0.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" style="35" customWidth="1"/>
-    <col min="4" max="5" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="33" customWidth="1"/>
+    <col min="4" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="0.42578125" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="27" customWidth="1"/>
-    <col min="8" max="9" width="14.5703125" customWidth="1"/>
+    <col min="8" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="0.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:19" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:19" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="55"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="55"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="29" t="s">
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="55"/>
-      <c r="C4" s="47" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="49" t="s">
+      <c r="D4" s="57"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="45"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="21"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="31"/>
+      <c r="S4" s="31"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="55"/>
-      <c r="C5" s="36" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="40" t="s">
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="45"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="36"/>
       <c r="K5" s="21"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="32"/>
-      <c r="S5" s="32"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="55"/>
-      <c r="C6" s="36" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="40" t="s">
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="45"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="36"/>
       <c r="K6" s="21"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-      <c r="P6" s="32"/>
-      <c r="Q6" s="32"/>
-      <c r="R6" s="32"/>
-      <c r="S6" s="32"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="31"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="55"/>
-      <c r="C7" s="36" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="40" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="45"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="36"/>
       <c r="K7" s="21"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="32"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="55"/>
-      <c r="C8" s="36" t="s">
+      <c r="B8" s="43"/>
+      <c r="C8" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="33" t="s">
+      <c r="D8" s="48"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="45"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="36"/>
       <c r="K8" s="21"/>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="30"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="32"/>
-      <c r="R8" s="32"/>
-      <c r="S8" s="32"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="55"/>
-      <c r="C9" s="36" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="33" t="s">
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="31"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="30"/>
       <c r="K9" s="21"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
-      <c r="C10" s="42" t="s">
+      <c r="B10" s="43"/>
+      <c r="C10" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="42" t="s">
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="46"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="32"/>
-      <c r="P10" s="32"/>
-      <c r="Q10" s="32"/>
-      <c r="R10" s="32"/>
-      <c r="S10" s="32"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="55"/>
-      <c r="C11" s="36" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="40" t="s">
+      <c r="D11" s="48"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="32"/>
-      <c r="S11" s="32"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B12" s="55"/>
-      <c r="C12" s="36" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="40" t="s">
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="30"/>
-      <c r="L12" s="32"/>
-      <c r="M12" s="32"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="32"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="32"/>
-      <c r="S12" s="32"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
-      <c r="C13" s="36" t="s">
+      <c r="B13" s="43"/>
+      <c r="C13" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="40" t="s">
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="46"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
+      <c r="H13" s="48"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
-      <c r="C14" s="36" t="s">
+      <c r="B14" s="43"/>
+      <c r="C14" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="40" t="s">
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="30"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
+      <c r="H14" s="48"/>
+      <c r="I14" s="48"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B15" s="55"/>
-      <c r="C15" s="36" t="s">
+      <c r="B15" s="43"/>
+      <c r="C15" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="40" t="s">
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="46"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="37"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
@@ -2570,217 +2579,259 @@
       <c r="S15" s="21"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="43" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="43" t="s">
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="55"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
-      <c r="C17" s="36" t="s">
+      <c r="B17" s="43"/>
+      <c r="C17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="40" t="s">
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="55"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="43"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="55"/>
-      <c r="C18" s="36" t="s">
+      <c r="B18" s="43"/>
+      <c r="C18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="40" t="s">
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="55"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="43"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="55"/>
-      <c r="C19" s="36" t="s">
+      <c r="B19" s="43"/>
+      <c r="C19" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="40" t="s">
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="55"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="55"/>
-      <c r="C20" s="36" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="40" t="s">
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="55"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="55"/>
-      <c r="C21" s="36" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="40" t="s">
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="55"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="43"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="55"/>
-      <c r="C22" s="44" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="44" t="s">
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="57"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="44"/>
       <c r="K22" s="27"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="55"/>
-      <c r="C23" s="36" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="40" t="s">
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="57"/>
+      <c r="H23" s="48"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="44"/>
       <c r="K23" s="27"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="55"/>
-      <c r="C24" s="36" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="40" t="s">
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="57"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="44"/>
       <c r="K24" s="27"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="55"/>
-      <c r="C25" s="36" t="s">
+      <c r="B25" s="43"/>
+      <c r="C25" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="40" t="s">
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="57"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="44"/>
       <c r="K25" s="27"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="55"/>
-      <c r="C26" s="36" t="s">
+      <c r="B26" s="43"/>
+      <c r="C26" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="40" t="s">
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="57"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="44"/>
       <c r="K26" s="27"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="55"/>
-      <c r="C27" s="50" t="s">
+      <c r="B27" s="43"/>
+      <c r="C27" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="52" t="s">
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="51"/>
-      <c r="I27" s="51"/>
-      <c r="J27" s="57"/>
+      <c r="H27" s="47"/>
+      <c r="I27" s="47"/>
+      <c r="J27" s="44"/>
       <c r="K27" s="27"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
-      <c r="C28" s="53" t="s">
+      <c r="B28" s="43"/>
+      <c r="C28" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="55"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="2:11" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="H29" s="56"/>
-      <c r="I29" s="56"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="D28:I28"/>
     <mergeCell ref="H27:I27"/>
     <mergeCell ref="H25:I25"/>
@@ -2791,48 +2842,6 @@
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
added experimental pointer to righthand controller
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Projects\Windows\SteamVR-Undistort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Windows\SteamVR-Undistort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A905752-D62A-4422-A146-274A0AB1BC11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40127CE-369C-472C-9999-3B968F22FD53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{6DC6B09A-E7DA-49A2-B7A4-0C67EEFD1649}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
   <si>
     <t>width</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>Adjust Step</t>
+  </si>
+  <si>
+    <t>Z Right</t>
   </si>
 </sst>
 </file>
@@ -505,44 +508,44 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -863,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A7B1EB-79F9-4052-A890-3A2B4DC96661}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J60" sqref="J60"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="O37" s="13" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
@@ -1771,8 +1774,8 @@
         <v>1.1111111111111092</v>
       </c>
       <c r="E41">
-        <f>G6/G41</f>
-        <v>0.62499995672727382</v>
+        <f>G41/G6</f>
+        <v>1.6000001107781867</v>
       </c>
       <c r="G41" s="4">
         <v>1.2222222222222201</v>
@@ -1795,8 +1798,8 @@
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E42">
-        <f>H7/H42</f>
-        <v>0.62500005454545449</v>
+        <f>H42/H7</f>
+        <v>1.5999998603636487</v>
       </c>
       <c r="G42" s="4">
         <v>0</v>
@@ -1840,13 +1843,13 @@
     <row r="44" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E44">
         <f>I41*E41</f>
-        <v>-5.5808993849017413E-2</v>
+        <v>-0.1428710440372265</v>
       </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E45">
         <f>I42*E42</f>
-        <v>1.4024659818250641E-3</v>
+        <v>3.5903122867994475E-3</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>52</v>
@@ -1868,7 +1871,7 @@
       </c>
       <c r="P45">
         <f>N41*E42</f>
-        <v>5.7267169809353591E-2</v>
+        <v>0.14660392912289466</v>
       </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.25">
@@ -1892,7 +1895,7 @@
       </c>
       <c r="P46">
         <f>N42*E42</f>
-        <v>-4.6270723069043781E-3</v>
+        <v>-1.1845303038131316E-2</v>
       </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.25">
@@ -2268,17 +2271,17 @@
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B3" s="43"/>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
       <c r="F3" s="42"/>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="44"/>
       <c r="K3" s="31"/>
       <c r="L3" s="31"/>
@@ -2295,14 +2298,14 @@
       <c r="C4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
       <c r="F4" s="36"/>
       <c r="G4" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
       <c r="J4" s="36"/>
       <c r="K4" s="21"/>
       <c r="L4" s="31"/>
@@ -2319,14 +2322,14 @@
       <c r="C5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="36"/>
       <c r="G5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="36"/>
       <c r="K5" s="21"/>
       <c r="L5" s="31"/>
@@ -2343,14 +2346,14 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
       <c r="F6" s="36"/>
       <c r="G6" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
       <c r="J6" s="36"/>
       <c r="K6" s="21"/>
       <c r="L6" s="31"/>
@@ -2367,14 +2370,14 @@
       <c r="C7" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
       <c r="F7" s="36"/>
       <c r="G7" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="54"/>
-      <c r="I7" s="54"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
       <c r="J7" s="36"/>
       <c r="K7" s="21"/>
       <c r="L7" s="31"/>
@@ -2391,14 +2394,14 @@
       <c r="C8" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
       <c r="F8" s="30"/>
       <c r="G8" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
       <c r="J8" s="36"/>
       <c r="K8" s="21"/>
       <c r="L8" s="31"/>
@@ -2415,14 +2418,14 @@
       <c r="C9" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
       <c r="F9" s="30"/>
       <c r="G9" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
       <c r="J9" s="30"/>
       <c r="K9" s="21"/>
       <c r="L9" s="29"/>
@@ -2436,17 +2439,17 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="43"/>
-      <c r="C10" s="56" t="s">
+      <c r="C10" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="37"/>
-      <c r="G10" s="56" t="s">
+      <c r="G10" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="37"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -2463,14 +2466,14 @@
       <c r="C11" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
       <c r="F11" s="37"/>
       <c r="G11" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
       <c r="J11" s="37"/>
       <c r="K11" s="29"/>
       <c r="L11" s="31"/>
@@ -2487,14 +2490,14 @@
       <c r="C12" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
       <c r="F12" s="37"/>
       <c r="G12" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
+      <c r="H12" s="47"/>
+      <c r="I12" s="47"/>
       <c r="J12" s="37"/>
       <c r="K12" s="29"/>
       <c r="L12" s="31"/>
@@ -2511,14 +2514,14 @@
       <c r="C13" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="37"/>
       <c r="G13" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
       <c r="J13" s="37"/>
       <c r="K13" s="29"/>
       <c r="L13" s="31"/>
@@ -2535,14 +2538,14 @@
       <c r="C14" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="37"/>
       <c r="G14" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
+      <c r="H14" s="47"/>
+      <c r="I14" s="47"/>
       <c r="J14" s="37"/>
       <c r="K14" s="29"/>
       <c r="L14" s="31"/>
@@ -2559,14 +2562,14 @@
       <c r="C15" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="37"/>
       <c r="G15" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="57"/>
       <c r="J15" s="37"/>
       <c r="K15" s="21"/>
       <c r="L15" s="21"/>
@@ -2580,17 +2583,17 @@
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="43"/>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="37"/>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
       <c r="J16" s="43"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -2598,14 +2601,14 @@
       <c r="C17" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="37"/>
       <c r="G17" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="43"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -2613,14 +2616,14 @@
       <c r="C18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
       <c r="F18" s="37"/>
       <c r="G18" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
       <c r="J18" s="43"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -2628,14 +2631,14 @@
       <c r="C19" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="37"/>
       <c r="G19" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
       <c r="J19" s="43"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -2643,14 +2646,14 @@
       <c r="C20" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="37"/>
       <c r="G20" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
       <c r="J20" s="43"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -2658,29 +2661,29 @@
       <c r="C21" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
       <c r="F21" s="37"/>
       <c r="G21" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
       <c r="J21" s="43"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="43"/>
-      <c r="C22" s="53" t="s">
+      <c r="C22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
       <c r="F22" s="37"/>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
       <c r="J22" s="44"/>
       <c r="K22" s="27"/>
     </row>
@@ -2689,14 +2692,14 @@
       <c r="C23" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
       <c r="F23" s="37"/>
       <c r="G23" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
       <c r="J23" s="44"/>
       <c r="K23" s="27"/>
     </row>
@@ -2705,14 +2708,14 @@
       <c r="C24" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
       <c r="F24" s="37"/>
       <c r="G24" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
       <c r="J24" s="44"/>
       <c r="K24" s="27"/>
     </row>
@@ -2721,14 +2724,14 @@
       <c r="C25" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
       <c r="F25" s="37"/>
       <c r="G25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
       <c r="J25" s="44"/>
       <c r="K25" s="27"/>
     </row>
@@ -2737,14 +2740,14 @@
       <c r="C26" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
       <c r="F26" s="37"/>
       <c r="G26" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
       <c r="J26" s="44"/>
       <c r="K26" s="27"/>
     </row>
@@ -2753,20 +2756,20 @@
       <c r="C27" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="37"/>
       <c r="G27" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="H27" s="47"/>
-      <c r="I27" s="47"/>
+      <c r="H27" s="58"/>
+      <c r="I27" s="58"/>
       <c r="J27" s="44"/>
       <c r="K27" s="27"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="43"/>
-      <c r="C28" s="58" t="s">
+      <c r="C28" s="46" t="s">
         <v>67</v>
       </c>
       <c r="D28" s="59"/>
@@ -2779,24 +2782,46 @@
     </row>
     <row r="29" spans="2:11" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="43"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
       <c r="J29" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="D28:I28"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="H17:I17"/>
     <mergeCell ref="H11:I11"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="D4:E4"/>
@@ -2813,35 +2838,13 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D28:I28"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated scratchpad for approximate focal pixel lenght calculation
</commit_message>
<xml_diff>
--- a/Parameters.xlsx
+++ b/Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Windows\SteamVR-Undistort\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40127CE-369C-472C-9999-3B968F22FD53}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB321659-570E-4315-BF7F-8FBF4C56881A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{6DC6B09A-E7DA-49A2-B7A4-0C67EEFD1649}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
   <si>
     <t>width</t>
   </si>
@@ -233,6 +233,36 @@
   </si>
   <si>
     <t>Z Right</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>1/f</t>
+  </si>
+  <si>
+    <t>1/d2</t>
+  </si>
+  <si>
+    <t>1/d1</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>d1</t>
+  </si>
+  <si>
+    <t>gear</t>
+  </si>
+  <si>
+    <t>vive</t>
   </si>
 </sst>
 </file>
@@ -523,14 +553,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -866,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10A7B1EB-79F9-4052-A890-3A2B4DC96661}">
   <dimension ref="A1:T67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,11 +946,18 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <v>1080</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="21">
+        <v>1200</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1194,7 +1231,10 @@
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B12" s="27"/>
       <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="D12" s="27">
+        <f>B3/B4</f>
+        <v>0.9</v>
+      </c>
       <c r="E12" s="27"/>
       <c r="G12" s="8">
         <v>0</v>
@@ -1236,7 +1276,10 @@
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="D13" s="26">
+        <f>B1/B2</f>
+        <v>0.89983164983164987</v>
+      </c>
       <c r="E13" s="26"/>
       <c r="G13" s="8">
         <v>0</v>
@@ -1266,7 +1309,10 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B14" s="26"/>
       <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
+      <c r="D14" s="26">
+        <f>H7/G6</f>
+        <v>0.90000014085819147</v>
+      </c>
       <c r="E14" s="26"/>
       <c r="G14" s="8">
         <v>0</v>
@@ -1296,7 +1342,10 @@
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="26">
+        <f>H42/G41</f>
+        <v>0.90000000000000169</v>
+      </c>
       <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1370,9 +1419,13 @@
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="E19" s="25"/>
       <c r="G19" s="8" t="s">
         <v>21</v>
@@ -1392,9 +1445,15 @@
       <c r="N19" s="21"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="B20" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="3">
+        <v>4.25</v>
+      </c>
+      <c r="D20" s="3">
+        <v>4.5</v>
+      </c>
       <c r="E20" s="25"/>
       <c r="G20" s="8" t="s">
         <v>13</v>
@@ -1414,9 +1473,15 @@
       <c r="N20" s="21"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3">
+        <v>25.75</v>
+      </c>
+      <c r="D21" s="3">
+        <v>25.5</v>
+      </c>
       <c r="E21" s="25"/>
       <c r="G21" s="8" t="s">
         <v>22</v>
@@ -1436,9 +1501,17 @@
       <c r="N21" s="21"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
+      <c r="B22" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="3">
+        <f>1/C20</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="D22" s="3">
+        <f>1/D20</f>
+        <v>0.22222222222222221</v>
+      </c>
       <c r="E22" s="25"/>
       <c r="G22" s="8" t="s">
         <v>23</v>
@@ -1458,9 +1531,17 @@
       <c r="N22" s="21"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
+      <c r="B23" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="3">
+        <f>1/C21</f>
+        <v>3.8834951456310676E-2</v>
+      </c>
+      <c r="D23" s="3">
+        <f>1/D21</f>
+        <v>3.9215686274509803E-2</v>
+      </c>
       <c r="E23" s="25"/>
       <c r="G23" s="8" t="s">
         <v>26</v>
@@ -1480,9 +1561,17 @@
       <c r="N23" s="21"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
+      <c r="B24" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="3">
+        <f>C22+C23</f>
+        <v>0.27412906910336948</v>
+      </c>
+      <c r="D24" s="3">
+        <f>D22+D23</f>
+        <v>0.26143790849673199</v>
+      </c>
       <c r="E24" s="25"/>
       <c r="G24" s="8" t="s">
         <v>25</v>
@@ -1502,9 +1591,17 @@
       <c r="N24" s="21"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
+      <c r="B25" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="3">
+        <f>1/C24</f>
+        <v>3.6479166666666671</v>
+      </c>
+      <c r="D25" s="3">
+        <f>1/D24</f>
+        <v>3.8250000000000006</v>
+      </c>
       <c r="E25" s="25"/>
       <c r="G25" s="8" t="s">
         <v>24</v>
@@ -1524,9 +1621,17 @@
       <c r="N25" s="21"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
+      <c r="B26" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="3">
+        <f>660/C25</f>
+        <v>180.92518560822384</v>
+      </c>
+      <c r="D26" s="3">
+        <f>C26</f>
+        <v>180.92518560822384</v>
+      </c>
       <c r="E26" s="25"/>
       <c r="G26" s="8" t="s">
         <v>27</v>
@@ -1546,9 +1651,17 @@
       <c r="N26" s="21"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="3">
+        <f>C26*C25</f>
+        <v>660</v>
+      </c>
+      <c r="D27" s="3">
+        <f>D26*D25</f>
+        <v>692.03883495145635</v>
+      </c>
       <c r="E27" s="25"/>
       <c r="G27" s="8" t="s">
         <v>28</v>
@@ -2298,14 +2411,14 @@
       <c r="C4" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="36"/>
       <c r="G4" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="36"/>
       <c r="K4" s="21"/>
       <c r="L4" s="31"/>
@@ -2322,14 +2435,14 @@
       <c r="C5" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
       <c r="F5" s="36"/>
       <c r="G5" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
       <c r="J5" s="36"/>
       <c r="K5" s="21"/>
       <c r="L5" s="31"/>
@@ -2346,14 +2459,14 @@
       <c r="C6" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="36"/>
       <c r="G6" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
       <c r="J6" s="36"/>
       <c r="K6" s="21"/>
       <c r="L6" s="31"/>
@@ -2370,14 +2483,14 @@
       <c r="C7" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
       <c r="F7" s="36"/>
       <c r="G7" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
       <c r="J7" s="36"/>
       <c r="K7" s="21"/>
       <c r="L7" s="31"/>
@@ -2439,17 +2552,17 @@
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="43"/>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
       <c r="F10" s="37"/>
-      <c r="G10" s="53" t="s">
+      <c r="G10" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
       <c r="J10" s="37"/>
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
@@ -2817,17 +2930,11 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="D28:I28"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="H9:I9"/>
     <mergeCell ref="G10:I10"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="H17:I17"/>
     <mergeCell ref="H11:I11"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="D11:E11"/>
@@ -2838,6 +2945,12 @@
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H9:I9"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>

</xml_diff>